<commit_message>
add streivers's cp and sde question bank
</commit_message>
<xml_diff>
--- a/Comp pro qus and sol/FINAL500.xlsx
+++ b/Comp pro qus and sol/FINAL500.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Truth\Problem Solving\question bank\Comp pro qus and sol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807FA016-895A-4060-A60D-63049A8B542A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E52C36B-27D2-42C6-BE9D-C91BC114AA6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="500">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1513,6 +1513,18 @@
   </si>
   <si>
     <t>stack</t>
+  </si>
+  <si>
+    <t>nearest greater left</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Equal Subset Sum in array T/F</t>
+  </si>
+  <si>
+    <t>if sum is odd the False</t>
   </si>
 </sst>
 </file>
@@ -1963,10 +1975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:D510"/>
+  <dimension ref="A1:D511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="B354" sqref="B354"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5669,16 +5681,21 @@
         <v>495</v>
       </c>
     </row>
-    <row r="353" spans="1:3" ht="21">
+    <row r="353" spans="1:4" ht="21">
       <c r="A353" s="5" t="s">
         <v>283</v>
       </c>
       <c r="B353" s="6" t="s">
         <v>487</v>
       </c>
-      <c r="C353" s="4"/>
-    </row>
-    <row r="354" spans="1:3" ht="21">
+      <c r="C353" s="11" t="s">
+        <v>463</v>
+      </c>
+      <c r="D353" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="354" spans="1:4" ht="21">
       <c r="A354" s="5" t="s">
         <v>283</v>
       </c>
@@ -5687,7 +5704,7 @@
       </c>
       <c r="C354" s="4"/>
     </row>
-    <row r="355" spans="1:3" ht="21">
+    <row r="355" spans="1:4" ht="21">
       <c r="A355" s="5" t="s">
         <v>283</v>
       </c>
@@ -5696,7 +5713,7 @@
       </c>
       <c r="C355" s="4"/>
     </row>
-    <row r="356" spans="1:3" ht="21">
+    <row r="356" spans="1:4" ht="21">
       <c r="A356" s="5" t="s">
         <v>283</v>
       </c>
@@ -5705,7 +5722,7 @@
       </c>
       <c r="C356" s="4"/>
     </row>
-    <row r="357" spans="1:3" ht="21">
+    <row r="357" spans="1:4" ht="21">
       <c r="A357" s="5" t="s">
         <v>283</v>
       </c>
@@ -5714,7 +5731,7 @@
       </c>
       <c r="C357" s="4"/>
     </row>
-    <row r="358" spans="1:3" ht="21">
+    <row r="358" spans="1:4" ht="21">
       <c r="A358" s="5" t="s">
         <v>283</v>
       </c>
@@ -5723,7 +5740,7 @@
       </c>
       <c r="C358" s="4"/>
     </row>
-    <row r="359" spans="1:3" ht="21">
+    <row r="359" spans="1:4" ht="21">
       <c r="A359" s="5" t="s">
         <v>283</v>
       </c>
@@ -5732,7 +5749,7 @@
       </c>
       <c r="C359" s="4"/>
     </row>
-    <row r="360" spans="1:3" ht="21">
+    <row r="360" spans="1:4" ht="21">
       <c r="A360" s="5" t="s">
         <v>283</v>
       </c>
@@ -5741,7 +5758,7 @@
       </c>
       <c r="C360" s="4"/>
     </row>
-    <row r="361" spans="1:3" ht="21">
+    <row r="361" spans="1:4" ht="21">
       <c r="A361" s="5" t="s">
         <v>283</v>
       </c>
@@ -5750,7 +5767,7 @@
       </c>
       <c r="C361" s="4"/>
     </row>
-    <row r="362" spans="1:3" ht="21">
+    <row r="362" spans="1:4" ht="21">
       <c r="A362" s="5" t="s">
         <v>283</v>
       </c>
@@ -5759,15 +5776,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="363" spans="1:3" ht="21">
+    <row r="363" spans="1:4" ht="21">
       <c r="B363" s="7"/>
       <c r="C363" s="4"/>
     </row>
-    <row r="364" spans="1:3" ht="21">
+    <row r="364" spans="1:4" ht="21">
       <c r="B364" s="7"/>
       <c r="C364" s="4"/>
     </row>
-    <row r="365" spans="1:3" ht="21">
+    <row r="365" spans="1:4" ht="21">
       <c r="A365" s="8" t="s">
         <v>320</v>
       </c>
@@ -5778,7 +5795,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="366" spans="1:3" ht="21">
+    <row r="366" spans="1:4" ht="21">
       <c r="A366" s="8" t="s">
         <v>320</v>
       </c>
@@ -5789,7 +5806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="367" spans="1:3" ht="21">
+    <row r="367" spans="1:4" ht="21">
       <c r="A367" s="8" t="s">
         <v>320</v>
       </c>
@@ -5800,7 +5817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="368" spans="1:3" ht="21">
+    <row r="368" spans="1:4" ht="21">
       <c r="A368" s="8" t="s">
         <v>320</v>
       </c>
@@ -6487,7 +6504,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="433" spans="1:3" ht="21">
+    <row r="433" spans="1:4" ht="21">
       <c r="A433" s="8" t="s">
         <v>383</v>
       </c>
@@ -6498,7 +6515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="434" spans="1:3" ht="21">
+    <row r="434" spans="1:4" ht="21">
       <c r="A434" s="8" t="s">
         <v>383</v>
       </c>
@@ -6509,7 +6526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="435" spans="1:3" ht="21">
+    <row r="435" spans="1:4" ht="21">
       <c r="A435" s="8" t="s">
         <v>383</v>
       </c>
@@ -6520,7 +6537,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="436" spans="1:3" ht="21">
+    <row r="436" spans="1:4" ht="21">
       <c r="A436" s="8" t="s">
         <v>383</v>
       </c>
@@ -6531,15 +6548,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="437" spans="1:3" ht="21">
+    <row r="437" spans="1:4" ht="21">
       <c r="B437" s="7"/>
       <c r="C437" s="4"/>
     </row>
-    <row r="438" spans="1:3" ht="21">
+    <row r="438" spans="1:4" ht="21">
       <c r="B438" s="7"/>
       <c r="C438" s="4"/>
     </row>
-    <row r="439" spans="1:3" ht="21">
+    <row r="439" spans="1:4" ht="21">
       <c r="A439" s="5" t="s">
         <v>389</v>
       </c>
@@ -6550,18 +6567,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="440" spans="1:3" ht="21">
+    <row r="440" spans="1:4" ht="21">
       <c r="A440" s="5" t="s">
         <v>389</v>
       </c>
       <c r="B440" s="6" t="s">
         <v>391</v>
       </c>
-      <c r="C440" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="441" spans="1:3" ht="21">
+      <c r="C440" s="11" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4" ht="21">
       <c r="A441" s="5" t="s">
         <v>389</v>
       </c>
@@ -6572,7 +6589,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="442" spans="1:3" ht="21">
+    <row r="442" spans="1:4" ht="21">
       <c r="A442" s="5" t="s">
         <v>389</v>
       </c>
@@ -6583,7 +6600,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="443" spans="1:3" ht="21">
+    <row r="443" spans="1:4" ht="21">
       <c r="A443" s="5" t="s">
         <v>389</v>
       </c>
@@ -6594,7 +6611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="444" spans="1:3" ht="21">
+    <row r="444" spans="1:4" ht="21">
       <c r="A444" s="5" t="s">
         <v>389</v>
       </c>
@@ -6605,7 +6622,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="445" spans="1:3" ht="21">
+    <row r="445" spans="1:4" ht="21">
       <c r="A445" s="5" t="s">
         <v>389</v>
       </c>
@@ -6616,34 +6633,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="446" spans="1:3" ht="21">
+    <row r="446" spans="1:4" ht="21">
       <c r="A446" s="5" t="s">
         <v>389</v>
       </c>
       <c r="B446" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="C446" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="447" spans="1:3" ht="21">
+        <v>498</v>
+      </c>
+      <c r="C446" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="D446" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" ht="21">
       <c r="A447" s="5" t="s">
         <v>389</v>
       </c>
       <c r="B447" s="6" t="s">
-        <v>397</v>
-      </c>
-      <c r="C447" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="448" spans="1:3" ht="21">
+        <v>271</v>
+      </c>
+      <c r="C447" s="11" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" ht="21">
       <c r="A448" s="5" t="s">
         <v>389</v>
       </c>
       <c r="B448" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C448" s="4" t="s">
         <v>4</v>
@@ -6654,7 +6674,7 @@
         <v>389</v>
       </c>
       <c r="B449" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C449" s="4" t="s">
         <v>4</v>
@@ -6665,7 +6685,7 @@
         <v>389</v>
       </c>
       <c r="B450" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C450" s="4" t="s">
         <v>4</v>
@@ -6676,7 +6696,7 @@
         <v>389</v>
       </c>
       <c r="B451" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C451" s="4" t="s">
         <v>4</v>
@@ -6687,7 +6707,7 @@
         <v>389</v>
       </c>
       <c r="B452" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C452" s="4" t="s">
         <v>4</v>
@@ -6698,7 +6718,7 @@
         <v>389</v>
       </c>
       <c r="B453" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C453" s="4" t="s">
         <v>4</v>
@@ -6709,7 +6729,7 @@
         <v>389</v>
       </c>
       <c r="B454" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C454" s="4" t="s">
         <v>4</v>
@@ -6720,7 +6740,7 @@
         <v>389</v>
       </c>
       <c r="B455" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C455" s="4" t="s">
         <v>4</v>
@@ -6731,7 +6751,7 @@
         <v>389</v>
       </c>
       <c r="B456" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C456" s="4" t="s">
         <v>4</v>
@@ -6742,7 +6762,7 @@
         <v>389</v>
       </c>
       <c r="B457" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C457" s="4" t="s">
         <v>4</v>
@@ -6753,7 +6773,7 @@
         <v>389</v>
       </c>
       <c r="B458" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C458" s="4" t="s">
         <v>4</v>
@@ -6764,7 +6784,7 @@
         <v>389</v>
       </c>
       <c r="B459" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C459" s="4" t="s">
         <v>4</v>
@@ -6775,7 +6795,7 @@
         <v>389</v>
       </c>
       <c r="B460" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C460" s="4" t="s">
         <v>4</v>
@@ -6786,7 +6806,7 @@
         <v>389</v>
       </c>
       <c r="B461" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C461" s="4" t="s">
         <v>4</v>
@@ -6797,7 +6817,7 @@
         <v>389</v>
       </c>
       <c r="B462" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C462" s="4" t="s">
         <v>4</v>
@@ -6808,7 +6828,7 @@
         <v>389</v>
       </c>
       <c r="B463" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C463" s="4" t="s">
         <v>4</v>
@@ -6819,7 +6839,7 @@
         <v>389</v>
       </c>
       <c r="B464" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C464" s="4" t="s">
         <v>4</v>
@@ -6830,7 +6850,7 @@
         <v>389</v>
       </c>
       <c r="B465" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C465" s="4" t="s">
         <v>4</v>
@@ -6841,7 +6861,7 @@
         <v>389</v>
       </c>
       <c r="B466" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C466" s="4" t="s">
         <v>4</v>
@@ -6852,7 +6872,7 @@
         <v>389</v>
       </c>
       <c r="B467" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C467" s="4" t="s">
         <v>4</v>
@@ -6863,7 +6883,7 @@
         <v>389</v>
       </c>
       <c r="B468" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C468" s="4" t="s">
         <v>4</v>
@@ -6874,7 +6894,7 @@
         <v>389</v>
       </c>
       <c r="B469" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C469" s="4" t="s">
         <v>4</v>
@@ -6885,7 +6905,7 @@
         <v>389</v>
       </c>
       <c r="B470" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C470" s="4" t="s">
         <v>4</v>
@@ -6896,7 +6916,7 @@
         <v>389</v>
       </c>
       <c r="B471" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C471" s="4" t="s">
         <v>4</v>
@@ -6907,7 +6927,7 @@
         <v>389</v>
       </c>
       <c r="B472" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C472" s="4" t="s">
         <v>4</v>
@@ -6918,7 +6938,7 @@
         <v>389</v>
       </c>
       <c r="B473" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C473" s="4" t="s">
         <v>4</v>
@@ -6929,7 +6949,7 @@
         <v>389</v>
       </c>
       <c r="B474" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C474" s="4" t="s">
         <v>4</v>
@@ -6940,7 +6960,7 @@
         <v>389</v>
       </c>
       <c r="B475" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C475" s="4" t="s">
         <v>4</v>
@@ -6951,7 +6971,7 @@
         <v>389</v>
       </c>
       <c r="B476" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C476" s="4" t="s">
         <v>4</v>
@@ -6962,7 +6982,7 @@
         <v>389</v>
       </c>
       <c r="B477" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C477" s="4" t="s">
         <v>4</v>
@@ -6973,7 +6993,7 @@
         <v>389</v>
       </c>
       <c r="B478" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C478" s="4" t="s">
         <v>4</v>
@@ -6984,7 +7004,7 @@
         <v>389</v>
       </c>
       <c r="B479" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C479" s="4" t="s">
         <v>4</v>
@@ -6995,7 +7015,7 @@
         <v>389</v>
       </c>
       <c r="B480" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C480" s="4" t="s">
         <v>4</v>
@@ -7006,7 +7026,7 @@
         <v>389</v>
       </c>
       <c r="B481" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C481" s="4" t="s">
         <v>4</v>
@@ -7017,7 +7037,7 @@
         <v>389</v>
       </c>
       <c r="B482" s="6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C482" s="4" t="s">
         <v>4</v>
@@ -7028,7 +7048,7 @@
         <v>389</v>
       </c>
       <c r="B483" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C483" s="4" t="s">
         <v>4</v>
@@ -7039,7 +7059,7 @@
         <v>389</v>
       </c>
       <c r="B484" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C484" s="4" t="s">
         <v>4</v>
@@ -7050,7 +7070,7 @@
         <v>389</v>
       </c>
       <c r="B485" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C485" s="4" t="s">
         <v>4</v>
@@ -7061,7 +7081,7 @@
         <v>389</v>
       </c>
       <c r="B486" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C486" s="4" t="s">
         <v>4</v>
@@ -7072,7 +7092,7 @@
         <v>389</v>
       </c>
       <c r="B487" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C487" s="4" t="s">
         <v>4</v>
@@ -7083,7 +7103,7 @@
         <v>389</v>
       </c>
       <c r="B488" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C488" s="4" t="s">
         <v>4</v>
@@ -7094,7 +7114,7 @@
         <v>389</v>
       </c>
       <c r="B489" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C489" s="4" t="s">
         <v>4</v>
@@ -7105,7 +7125,7 @@
         <v>389</v>
       </c>
       <c r="B490" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C490" s="4" t="s">
         <v>4</v>
@@ -7116,7 +7136,7 @@
         <v>389</v>
       </c>
       <c r="B491" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C491" s="4" t="s">
         <v>4</v>
@@ -7127,7 +7147,7 @@
         <v>389</v>
       </c>
       <c r="B492" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C492" s="4" t="s">
         <v>4</v>
@@ -7138,7 +7158,7 @@
         <v>389</v>
       </c>
       <c r="B493" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C493" s="4" t="s">
         <v>4</v>
@@ -7149,7 +7169,7 @@
         <v>389</v>
       </c>
       <c r="B494" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C494" s="4" t="s">
         <v>4</v>
@@ -7160,7 +7180,7 @@
         <v>389</v>
       </c>
       <c r="B495" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C495" s="4" t="s">
         <v>4</v>
@@ -7171,7 +7191,7 @@
         <v>389</v>
       </c>
       <c r="B496" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C496" s="4" t="s">
         <v>4</v>
@@ -7182,7 +7202,7 @@
         <v>389</v>
       </c>
       <c r="B497" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C497" s="4" t="s">
         <v>4</v>
@@ -7193,38 +7213,38 @@
         <v>389</v>
       </c>
       <c r="B498" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="C498" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="499" spans="1:3" ht="21">
+      <c r="A499" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="B499" s="6" t="s">
         <v>448</v>
       </c>
-      <c r="C498" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="499" spans="1:3" ht="21">
-      <c r="B499" s="7"/>
-      <c r="C499" s="4"/>
+      <c r="C499" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="500" spans="1:3" ht="21">
-      <c r="A500" s="8"/>
       <c r="B500" s="7"/>
       <c r="C500" s="4"/>
     </row>
     <row r="501" spans="1:3" ht="21">
-      <c r="A501" s="5" t="s">
-        <v>449</v>
-      </c>
-      <c r="B501" s="6" t="s">
-        <v>450</v>
-      </c>
-      <c r="C501" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A501" s="8"/>
+      <c r="B501" s="7"/>
+      <c r="C501" s="4"/>
     </row>
     <row r="502" spans="1:3" ht="21">
       <c r="A502" s="5" t="s">
         <v>449</v>
       </c>
       <c r="B502" s="6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C502" s="4" t="s">
         <v>4</v>
@@ -7235,7 +7255,7 @@
         <v>449</v>
       </c>
       <c r="B503" s="6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C503" s="4" t="s">
         <v>4</v>
@@ -7246,7 +7266,7 @@
         <v>449</v>
       </c>
       <c r="B504" s="6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C504" s="4" t="s">
         <v>4</v>
@@ -7257,7 +7277,7 @@
         <v>449</v>
       </c>
       <c r="B505" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C505" s="4" t="s">
         <v>4</v>
@@ -7268,7 +7288,7 @@
         <v>449</v>
       </c>
       <c r="B506" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C506" s="4" t="s">
         <v>4</v>
@@ -7279,7 +7299,7 @@
         <v>449</v>
       </c>
       <c r="B507" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C507" s="4" t="s">
         <v>4</v>
@@ -7290,7 +7310,7 @@
         <v>449</v>
       </c>
       <c r="B508" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C508" s="4" t="s">
         <v>4</v>
@@ -7301,7 +7321,7 @@
         <v>449</v>
       </c>
       <c r="B509" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C509" s="4" t="s">
         <v>4</v>
@@ -7312,9 +7332,20 @@
         <v>449</v>
       </c>
       <c r="B510" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="C510" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="511" spans="1:3" ht="21">
+      <c r="A511" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="B511" s="6" t="s">
         <v>459</v>
       </c>
-      <c r="C510" s="4" t="s">
+      <c r="C511" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7698,69 +7729,69 @@
     <hyperlink ref="B443" r:id="rId376" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
     <hyperlink ref="B444" r:id="rId377" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
     <hyperlink ref="B445" r:id="rId378" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
-    <hyperlink ref="B446" r:id="rId379" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
-    <hyperlink ref="B447" r:id="rId380" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
-    <hyperlink ref="B448" r:id="rId381" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
-    <hyperlink ref="B449" r:id="rId382" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
-    <hyperlink ref="B450" r:id="rId383" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
-    <hyperlink ref="B451" r:id="rId384" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
-    <hyperlink ref="B452" r:id="rId385" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
-    <hyperlink ref="B453" r:id="rId386" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
-    <hyperlink ref="B454" r:id="rId387" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
-    <hyperlink ref="B455" r:id="rId388" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
-    <hyperlink ref="B456" r:id="rId389" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
-    <hyperlink ref="B457" r:id="rId390" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
-    <hyperlink ref="B458" r:id="rId391" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
-    <hyperlink ref="B459" r:id="rId392" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
-    <hyperlink ref="B460" r:id="rId393" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
-    <hyperlink ref="B461" r:id="rId394" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
-    <hyperlink ref="B462" r:id="rId395" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
-    <hyperlink ref="B463" r:id="rId396" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
-    <hyperlink ref="B464" r:id="rId397" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
-    <hyperlink ref="B465" r:id="rId398" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
-    <hyperlink ref="B466" r:id="rId399" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
-    <hyperlink ref="B467" r:id="rId400" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
-    <hyperlink ref="B468" r:id="rId401" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
-    <hyperlink ref="B469" r:id="rId402" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
-    <hyperlink ref="B470" r:id="rId403" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
-    <hyperlink ref="B471" r:id="rId404" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
-    <hyperlink ref="B472" r:id="rId405" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
-    <hyperlink ref="B473" r:id="rId406" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
-    <hyperlink ref="B474" r:id="rId407" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
-    <hyperlink ref="B475" r:id="rId408" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
-    <hyperlink ref="B476" r:id="rId409" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
-    <hyperlink ref="B477" r:id="rId410" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
-    <hyperlink ref="B478" r:id="rId411" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
-    <hyperlink ref="B480" r:id="rId412" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
-    <hyperlink ref="B479" r:id="rId413" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
-    <hyperlink ref="B481" r:id="rId414" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
-    <hyperlink ref="B482" r:id="rId415" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
-    <hyperlink ref="B483" r:id="rId416" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
-    <hyperlink ref="B484" r:id="rId417" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
-    <hyperlink ref="B485" r:id="rId418" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
-    <hyperlink ref="B486" r:id="rId419" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
-    <hyperlink ref="B487" r:id="rId420" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
-    <hyperlink ref="B488" r:id="rId421" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
-    <hyperlink ref="B489" r:id="rId422" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
-    <hyperlink ref="B490" r:id="rId423" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
-    <hyperlink ref="B491" r:id="rId424" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
-    <hyperlink ref="B498" r:id="rId425" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
-    <hyperlink ref="B497" r:id="rId426" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
-    <hyperlink ref="B496" r:id="rId427" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
-    <hyperlink ref="B495" r:id="rId428" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
-    <hyperlink ref="B494" r:id="rId429" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
-    <hyperlink ref="B493" r:id="rId430" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
-    <hyperlink ref="B492" r:id="rId431" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
-    <hyperlink ref="B501" r:id="rId432" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
-    <hyperlink ref="B502" r:id="rId433" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
-    <hyperlink ref="B503" r:id="rId434" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
-    <hyperlink ref="B504" r:id="rId435" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
-    <hyperlink ref="B505" r:id="rId436" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
-    <hyperlink ref="B506" r:id="rId437" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
-    <hyperlink ref="B507" r:id="rId438" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
-    <hyperlink ref="B510" r:id="rId439" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
-    <hyperlink ref="B508" r:id="rId440" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
-    <hyperlink ref="B509" r:id="rId441" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
+    <hyperlink ref="B447" r:id="rId379" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
+    <hyperlink ref="B448" r:id="rId380" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
+    <hyperlink ref="B449" r:id="rId381" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
+    <hyperlink ref="B450" r:id="rId382" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
+    <hyperlink ref="B451" r:id="rId383" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
+    <hyperlink ref="B452" r:id="rId384" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
+    <hyperlink ref="B453" r:id="rId385" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
+    <hyperlink ref="B454" r:id="rId386" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
+    <hyperlink ref="B455" r:id="rId387" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
+    <hyperlink ref="B456" r:id="rId388" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
+    <hyperlink ref="B457" r:id="rId389" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
+    <hyperlink ref="B458" r:id="rId390" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
+    <hyperlink ref="B459" r:id="rId391" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
+    <hyperlink ref="B460" r:id="rId392" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
+    <hyperlink ref="B461" r:id="rId393" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
+    <hyperlink ref="B462" r:id="rId394" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
+    <hyperlink ref="B463" r:id="rId395" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
+    <hyperlink ref="B464" r:id="rId396" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
+    <hyperlink ref="B465" r:id="rId397" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
+    <hyperlink ref="B466" r:id="rId398" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
+    <hyperlink ref="B467" r:id="rId399" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
+    <hyperlink ref="B468" r:id="rId400" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
+    <hyperlink ref="B469" r:id="rId401" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
+    <hyperlink ref="B470" r:id="rId402" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
+    <hyperlink ref="B471" r:id="rId403" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
+    <hyperlink ref="B472" r:id="rId404" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
+    <hyperlink ref="B473" r:id="rId405" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
+    <hyperlink ref="B474" r:id="rId406" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
+    <hyperlink ref="B475" r:id="rId407" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
+    <hyperlink ref="B476" r:id="rId408" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
+    <hyperlink ref="B477" r:id="rId409" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
+    <hyperlink ref="B478" r:id="rId410" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
+    <hyperlink ref="B479" r:id="rId411" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
+    <hyperlink ref="B481" r:id="rId412" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
+    <hyperlink ref="B480" r:id="rId413" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
+    <hyperlink ref="B482" r:id="rId414" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
+    <hyperlink ref="B483" r:id="rId415" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
+    <hyperlink ref="B484" r:id="rId416" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
+    <hyperlink ref="B485" r:id="rId417" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
+    <hyperlink ref="B486" r:id="rId418" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
+    <hyperlink ref="B487" r:id="rId419" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
+    <hyperlink ref="B488" r:id="rId420" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
+    <hyperlink ref="B489" r:id="rId421" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
+    <hyperlink ref="B490" r:id="rId422" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
+    <hyperlink ref="B491" r:id="rId423" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
+    <hyperlink ref="B492" r:id="rId424" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
+    <hyperlink ref="B499" r:id="rId425" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
+    <hyperlink ref="B498" r:id="rId426" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
+    <hyperlink ref="B497" r:id="rId427" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
+    <hyperlink ref="B496" r:id="rId428" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
+    <hyperlink ref="B495" r:id="rId429" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
+    <hyperlink ref="B494" r:id="rId430" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
+    <hyperlink ref="B493" r:id="rId431" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
+    <hyperlink ref="B502" r:id="rId432" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
+    <hyperlink ref="B503" r:id="rId433" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
+    <hyperlink ref="B504" r:id="rId434" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
+    <hyperlink ref="B505" r:id="rId435" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
+    <hyperlink ref="B506" r:id="rId436" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
+    <hyperlink ref="B507" r:id="rId437" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
+    <hyperlink ref="B508" r:id="rId438" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
+    <hyperlink ref="B511" r:id="rId439" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
+    <hyperlink ref="B509" r:id="rId440" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
+    <hyperlink ref="B510" r:id="rId441" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
     <hyperlink ref="B385" r:id="rId442" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
     <hyperlink ref="B49" r:id="rId443" xr:uid="{4B0AB152-2C4E-4C61-8143-54AD3B07F0ED}"/>
     <hyperlink ref="B51" r:id="rId444" xr:uid="{3ACBE086-2488-4747-A1D1-4CCBFAC5A269}"/>

</xml_diff>